<commit_message>
modified and create new.csv and new.xlsx
</commit_message>
<xml_diff>
--- a/new.xlsx
+++ b/new.xlsx
@@ -7,14 +7,14 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="stocks" sheetId="1" r:id="rId1"/>
+    <sheet name="stock" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>tickers</t>
   </si>
@@ -46,13 +46,10 @@
     <t>TATA</t>
   </si>
   <si>
-    <t>not available</t>
-  </si>
-  <si>
     <t>larry page</t>
   </si>
   <si>
-    <t>Sam Walton</t>
+    <t>Allif</t>
   </si>
   <si>
     <t>bill gates</t>
@@ -419,112 +416,121 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B3:F8"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="3" spans="2:6">
-      <c r="B3" s="1" t="s">
+    <row r="1" spans="1:6">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="2:6">
+    <row r="2" spans="1:6">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>27.82</v>
+      </c>
+      <c r="D2">
+        <v>87</v>
+      </c>
+      <c r="E2">
+        <v>845</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3">
+        <v>4.61</v>
+      </c>
+      <c r="D3">
+        <v>484</v>
+      </c>
+      <c r="E3">
+        <v>65</v>
+      </c>
+      <c r="F3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C4">
-        <v>27.82</v>
+        <v>-1</v>
       </c>
       <c r="D4">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E4">
-        <v>845</v>
+        <v>64</v>
       </c>
       <c r="F4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
-    <row r="5" spans="2:6">
+    <row r="5" spans="1:6">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
       <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5">
-        <v>4.61</v>
+        <v>8</v>
       </c>
       <c r="D5">
-        <v>484</v>
+        <v>50</v>
       </c>
       <c r="E5">
-        <v>65</v>
+        <v>1023</v>
       </c>
       <c r="F5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
-    <row r="6" spans="2:6">
+    <row r="6" spans="1:6">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C6">
+        <v>5.6</v>
+      </c>
+      <c r="D6">
         <v>-1</v>
       </c>
-      <c r="D6">
-        <v>85</v>
-      </c>
-      <c r="E6">
-        <v>64</v>
-      </c>
       <c r="F6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6">
-      <c r="B7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7">
-        <v>50</v>
-      </c>
-      <c r="E7">
-        <v>1023</v>
-      </c>
-      <c r="F7" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6">
-      <c r="B8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8">
-        <v>5.6</v>
-      </c>
-      <c r="D8">
-        <v>-1</v>
-      </c>
-      <c r="E8">
-        <v>50</v>
-      </c>
-      <c r="F8" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>